<commit_message>
added import from excel
</commit_message>
<xml_diff>
--- a/xlsFiles/test.xlsx
+++ b/xlsFiles/test.xlsx
@@ -67,7 +67,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:C51"/>
+  <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -83,134 +83,143 @@
       <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0">
+        <v>600</v>
+      </c>
+      <c r="E1" s="0">
+        <v>6</v>
+      </c>
+      <c r="F1" s="0">
+        <v>60</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B2" s="0">
         <v>348</v>
       </c>
       <c r="C2" s="0">
-        <v>487</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>304</v>
+        <v>426</v>
       </c>
       <c r="B3" s="0">
-        <v>375</v>
+        <v>475</v>
       </c>
       <c r="C3" s="0">
-        <v>421</v>
+        <v>121</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>364</v>
+        <v>200</v>
       </c>
       <c r="B4" s="0">
-        <v>346</v>
+        <v>246</v>
       </c>
       <c r="C4" s="0">
-        <v>422</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B5" s="0">
-        <v>129</v>
+        <v>29</v>
       </c>
       <c r="C5" s="0">
-        <v>360</v>
+        <v>260</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0">
-        <v>422</v>
+        <v>442</v>
       </c>
       <c r="B6" s="0">
-        <v>476</v>
+        <v>576</v>
       </c>
       <c r="C6" s="0">
-        <v>396</v>
+        <v>196</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0">
-        <v>358</v>
+        <v>409</v>
       </c>
       <c r="B7" s="0">
-        <v>291</v>
+        <v>391</v>
       </c>
       <c r="C7" s="0">
-        <v>8</v>
+        <v>408</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>271</v>
+        <v>244</v>
       </c>
       <c r="B8" s="0">
-        <v>114</v>
+        <v>314</v>
       </c>
       <c r="C8" s="0">
-        <v>120</v>
+        <v>520</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>383</v>
+        <v>488</v>
       </c>
       <c r="B9" s="0">
-        <v>441</v>
+        <v>241</v>
       </c>
       <c r="C9" s="0">
-        <v>44</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>22</v>
+        <v>394</v>
       </c>
       <c r="B10" s="0">
-        <v>424</v>
+        <v>124</v>
       </c>
       <c r="C10" s="0">
-        <v>219</v>
+        <v>519</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0">
-        <v>313</v>
+        <v>383</v>
       </c>
       <c r="B11" s="0">
-        <v>487</v>
+        <v>587</v>
       </c>
       <c r="C11" s="0">
-        <v>189</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0">
-        <v>429</v>
+        <v>176</v>
       </c>
       <c r="B12" s="0">
-        <v>326</v>
+        <v>526</v>
       </c>
       <c r="C12" s="0">
-        <v>307</v>
+        <v>507</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0">
-        <v>239</v>
+        <v>547</v>
       </c>
       <c r="B13" s="0">
-        <v>193</v>
+        <v>493</v>
       </c>
       <c r="C13" s="0">
         <v>222</v>
@@ -218,120 +227,120 @@
     </row>
     <row r="14">
       <c r="A14" s="0">
-        <v>282</v>
+        <v>538</v>
       </c>
       <c r="B14" s="0">
         <v>168</v>
       </c>
       <c r="C14" s="0">
-        <v>312</v>
+        <v>212</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0">
-        <v>214</v>
+        <v>70</v>
       </c>
       <c r="B15" s="0">
-        <v>299</v>
+        <v>599</v>
       </c>
       <c r="C15" s="0">
-        <v>313</v>
+        <v>513</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0">
-        <v>442</v>
+        <v>577</v>
       </c>
       <c r="B16" s="0">
         <v>138</v>
       </c>
       <c r="C16" s="0">
-        <v>279</v>
+        <v>479</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0">
-        <v>165</v>
+        <v>48</v>
       </c>
       <c r="B17" s="0">
-        <v>17</v>
+        <v>217</v>
       </c>
       <c r="C17" s="0">
-        <v>438</v>
+        <v>138</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0">
-        <v>262</v>
+        <v>547</v>
       </c>
       <c r="B18" s="0">
-        <v>492</v>
+        <v>292</v>
       </c>
       <c r="C18" s="0">
-        <v>58</v>
+        <v>358</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0">
-        <v>347</v>
+        <v>394</v>
       </c>
       <c r="B19" s="0">
-        <v>479</v>
+        <v>179</v>
       </c>
       <c r="C19" s="0">
-        <v>233</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0">
-        <v>292</v>
+        <v>165</v>
       </c>
       <c r="B20" s="0">
-        <v>246</v>
+        <v>46</v>
       </c>
       <c r="C20" s="0">
-        <v>202</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0">
-        <v>35</v>
+        <v>520</v>
       </c>
       <c r="B21" s="0">
         <v>77</v>
       </c>
       <c r="C21" s="0">
-        <v>108</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0">
-        <v>349</v>
+        <v>428</v>
       </c>
       <c r="B22" s="0">
-        <v>340</v>
+        <v>240</v>
       </c>
       <c r="C22" s="0">
-        <v>196</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0">
-        <v>459</v>
+        <v>368</v>
       </c>
       <c r="B23" s="0">
-        <v>267</v>
+        <v>567</v>
       </c>
       <c r="C23" s="0">
-        <v>104</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0">
-        <v>81</v>
+        <v>426</v>
       </c>
       <c r="B24" s="0">
-        <v>90</v>
+        <v>490</v>
       </c>
       <c r="C24" s="0">
         <v>128</v>
@@ -339,43 +348,43 @@
     </row>
     <row r="25">
       <c r="A25" s="0">
-        <v>76</v>
+        <v>557</v>
       </c>
       <c r="B25" s="0">
         <v>497</v>
       </c>
       <c r="C25" s="0">
-        <v>23</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="0">
-        <v>243</v>
+        <v>525</v>
       </c>
       <c r="B26" s="0">
-        <v>428</v>
+        <v>228</v>
       </c>
       <c r="C26" s="0">
-        <v>35</v>
+        <v>235</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="0">
-        <v>490</v>
+        <v>320</v>
       </c>
       <c r="B27" s="0">
-        <v>55</v>
+        <v>355</v>
       </c>
       <c r="C27" s="0">
-        <v>12</v>
+        <v>512</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="0">
-        <v>359</v>
+        <v>422</v>
       </c>
       <c r="B28" s="0">
-        <v>118</v>
+        <v>518</v>
       </c>
       <c r="C28" s="0">
         <v>341</v>
@@ -383,18 +392,18 @@
     </row>
     <row r="29">
       <c r="A29" s="0">
-        <v>108</v>
+        <v>28</v>
       </c>
       <c r="B29" s="0">
-        <v>361</v>
+        <v>61</v>
       </c>
       <c r="C29" s="0">
-        <v>122</v>
+        <v>422</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0">
-        <v>393</v>
+        <v>546</v>
       </c>
       <c r="B30" s="0">
         <v>40</v>
@@ -405,109 +414,109 @@
     </row>
     <row r="31">
       <c r="A31" s="0">
-        <v>258</v>
+        <v>294</v>
       </c>
       <c r="B31" s="0">
-        <v>95</v>
+        <v>295</v>
       </c>
       <c r="C31" s="0">
-        <v>408</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="0">
-        <v>468</v>
+        <v>193</v>
       </c>
       <c r="B32" s="0">
-        <v>110</v>
+        <v>210</v>
       </c>
       <c r="C32" s="0">
-        <v>364</v>
+        <v>564</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="0">
-        <v>286</v>
+        <v>526</v>
       </c>
       <c r="B33" s="0">
-        <v>361</v>
+        <v>561</v>
       </c>
       <c r="C33" s="0">
-        <v>224</v>
+        <v>524</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="0">
-        <v>356</v>
+        <v>291</v>
       </c>
       <c r="B34" s="0">
-        <v>240</v>
+        <v>340</v>
       </c>
       <c r="C34" s="0">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="0">
-        <v>111</v>
+        <v>255</v>
       </c>
       <c r="B35" s="0">
         <v>123</v>
       </c>
       <c r="C35" s="0">
-        <v>232</v>
+        <v>332</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="0">
-        <v>91</v>
+        <v>355</v>
       </c>
       <c r="B36" s="0">
-        <v>234</v>
+        <v>334</v>
       </c>
       <c r="C36" s="0">
-        <v>58</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="0">
-        <v>469</v>
+        <v>58</v>
       </c>
       <c r="B37" s="0">
-        <v>257</v>
+        <v>557</v>
       </c>
       <c r="C37" s="0">
-        <v>393</v>
+        <v>593</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="0">
-        <v>216</v>
+        <v>578</v>
       </c>
       <c r="B38" s="0">
-        <v>92</v>
+        <v>592</v>
       </c>
       <c r="C38" s="0">
-        <v>264</v>
+        <v>64</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="0">
-        <v>488</v>
+        <v>408</v>
       </c>
       <c r="B39" s="0">
-        <v>123</v>
+        <v>23</v>
       </c>
       <c r="C39" s="0">
-        <v>156</v>
+        <v>456</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="0">
-        <v>440</v>
+        <v>124</v>
       </c>
       <c r="B40" s="0">
-        <v>454</v>
+        <v>354</v>
       </c>
       <c r="C40" s="0">
         <v>143</v>
@@ -515,98 +524,98 @@
     </row>
     <row r="41">
       <c r="A41" s="0">
-        <v>29</v>
+        <v>565</v>
       </c>
       <c r="B41" s="0">
-        <v>221</v>
+        <v>521</v>
       </c>
       <c r="C41" s="0">
-        <v>364</v>
+        <v>164</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="0">
-        <v>47</v>
+        <v>428</v>
       </c>
       <c r="B42" s="0">
-        <v>368</v>
+        <v>468</v>
       </c>
       <c r="C42" s="0">
-        <v>284</v>
+        <v>484</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="0">
-        <v>168</v>
+        <v>495</v>
       </c>
       <c r="B43" s="0">
-        <v>383</v>
+        <v>483</v>
       </c>
       <c r="C43" s="0">
-        <v>166</v>
+        <v>366</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="0">
-        <v>175</v>
+        <v>571</v>
       </c>
       <c r="B44" s="0">
-        <v>210</v>
+        <v>110</v>
       </c>
       <c r="C44" s="0">
-        <v>415</v>
+        <v>315</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="0">
-        <v>367</v>
+        <v>231</v>
       </c>
       <c r="B45" s="0">
-        <v>81</v>
+        <v>581</v>
       </c>
       <c r="C45" s="0">
-        <v>172</v>
+        <v>372</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="0">
-        <v>83</v>
+        <v>187</v>
       </c>
       <c r="B46" s="0">
-        <v>212</v>
+        <v>312</v>
       </c>
       <c r="C46" s="0">
-        <v>315</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="0">
-        <v>3</v>
+        <v>468</v>
       </c>
       <c r="B47" s="0">
-        <v>327</v>
+        <v>527</v>
       </c>
       <c r="C47" s="0">
-        <v>242</v>
+        <v>142</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="0">
-        <v>370</v>
+        <v>513</v>
       </c>
       <c r="B48" s="0">
-        <v>46</v>
+        <v>546</v>
       </c>
       <c r="C48" s="0">
-        <v>5</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="0">
-        <v>466</v>
+        <v>499</v>
       </c>
       <c r="B49" s="0">
-        <v>429</v>
+        <v>329</v>
       </c>
       <c r="C49" s="0">
         <v>50</v>
@@ -614,10 +623,10 @@
     </row>
     <row r="50">
       <c r="A50" s="0">
-        <v>125</v>
+        <v>135</v>
       </c>
       <c r="B50" s="0">
-        <v>416</v>
+        <v>316</v>
       </c>
       <c r="C50" s="0">
         <v>25</v>
@@ -625,13 +634,123 @@
     </row>
     <row r="51">
       <c r="A51" s="0">
+        <v>391</v>
+      </c>
+      <c r="B51" s="0">
+        <v>139</v>
+      </c>
+      <c r="C51" s="0">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="0">
+        <v>410</v>
+      </c>
+      <c r="B52" s="0">
+        <v>582</v>
+      </c>
+      <c r="C52" s="0">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="0">
+        <v>198</v>
+      </c>
+      <c r="B53" s="0">
+        <v>117</v>
+      </c>
+      <c r="C53" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="0">
+        <v>390</v>
+      </c>
+      <c r="B54" s="0">
+        <v>432</v>
+      </c>
+      <c r="C54" s="0">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="0">
+        <v>279</v>
+      </c>
+      <c r="B55" s="0">
+        <v>47</v>
+      </c>
+      <c r="C55" s="0">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="0">
+        <v>401</v>
+      </c>
+      <c r="B56" s="0">
+        <v>42</v>
+      </c>
+      <c r="C56" s="0">
         <v>407</v>
       </c>
-      <c r="B51" s="0">
-        <v>239</v>
-      </c>
-      <c r="C51" s="0">
-        <v>6</v>
+    </row>
+    <row r="57">
+      <c r="A57" s="0">
+        <v>272</v>
+      </c>
+      <c r="B57" s="0">
+        <v>377</v>
+      </c>
+      <c r="C57" s="0">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="0">
+        <v>76</v>
+      </c>
+      <c r="B58" s="0">
+        <v>20</v>
+      </c>
+      <c r="C58" s="0">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="0">
+        <v>377</v>
+      </c>
+      <c r="B59" s="0">
+        <v>307</v>
+      </c>
+      <c r="C59" s="0">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="0">
+        <v>547</v>
+      </c>
+      <c r="B60" s="0">
+        <v>590</v>
+      </c>
+      <c r="C60" s="0">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="0">
+        <v>58</v>
+      </c>
+      <c r="B61" s="0">
+        <v>21</v>
+      </c>
+      <c r="C61" s="0">
+        <v>526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>